<commit_message>
Change required hours number for each group
</commit_message>
<xml_diff>
--- a/data/groups/group1_schedule.xlsx
+++ b/data/groups/group1_schedule.xlsx
@@ -1295,7 +1295,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1305,7 +1305,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1315,7 +1315,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1345,7 +1345,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1365,7 +1365,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>

</xml_diff>